<commit_message>
The last Home page
Alan Whitten
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v.1.2 Home Page.xlsx
+++ b/Testing Spreadsheet v.1.2 Home Page.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="A6C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16180" windowHeight="7860" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16180" windowHeight="7860" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Reqs" sheetId="5" r:id="rId1"/>
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="278">
   <si>
     <t xml:space="preserve">Req </t>
   </si>
@@ -999,12 +999,87 @@
   <si>
     <t>Amazon Kindle Fire 7 inch, iPad 4, iPhone 6, Google Nexus 10 and Samsung Galaxy S4, Google Chrome, Firefox, Internet Explorer.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Requirements 4.1.9 </t>
+  </si>
+  <si>
+    <t>From any web page all users of the system that are not logged in should be able to directly navigate to the Register and Log in pages.</t>
+  </si>
+  <si>
+    <t>Home_TConn_19</t>
+  </si>
+  <si>
+    <t>Home_TConn_20</t>
+  </si>
+  <si>
+    <t>Home_TConn_21</t>
+  </si>
+  <si>
+    <t>In addition all logged in users should be able to log off from any page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From any web page all users of the system that are logged in should be able to directly navigate to the My Account – reset password page. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirements 4.1.10 </t>
+  </si>
+  <si>
+    <t>T_Case_26</t>
+  </si>
+  <si>
+    <t>T_Case_27</t>
+  </si>
+  <si>
+    <t>T_Case_28</t>
+  </si>
+  <si>
+    <t>To show that from the Home page, a user can navigate directly to the Register and login pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check that from the Home page users that are logged in are able to directly navigate to the My Account – reset password page. </t>
+  </si>
+  <si>
+    <t>Check that from the Home page logged in users are able to log off from any page.</t>
+  </si>
+  <si>
+    <t>Home_Tproc_27</t>
+  </si>
+  <si>
+    <t>Home_Tproc_28</t>
+  </si>
+  <si>
+    <t>While on the Home page when the register tab is clicked.</t>
+  </si>
+  <si>
+    <t>The Register page is displayed.</t>
+  </si>
+  <si>
+    <t>While on the Home page when the Loigin tab is clicked.</t>
+  </si>
+  <si>
+    <t>While on the Home page and logged in, when the username in the top right is clicked.</t>
+  </si>
+  <si>
+    <t>The My Account – reset password page. Is displayed.</t>
+  </si>
+  <si>
+    <t>Home_Tproc_29</t>
+  </si>
+  <si>
+    <t>Home_Tproc_30</t>
+  </si>
+  <si>
+    <t>While on the Home page and looged in, when the log off tab is clikcked</t>
+  </si>
+  <si>
+    <t>The user is logged off</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1102,6 +1177,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1190,7 +1272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1296,6 +1378,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1443,7 +1531,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -1539,10 +1627,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1566,11 +1654,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="260253296"/>
-        <c:axId val="260256824"/>
+        <c:axId val="283541136"/>
+        <c:axId val="283542704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260253296"/>
+        <c:axId val="283541136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1580,7 +1668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260256824"/>
+        <c:crossAx val="283542704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1588,7 +1676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260256824"/>
+        <c:axId val="283542704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,7 +1687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260253296"/>
+        <c:crossAx val="283541136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2026,10 +2114,10 @@
   <sheetPr>
     <tabColor rgb="FF023FAE"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A13" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2321,9 +2409,52 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="D20" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="38" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2352,8 +2483,8 @@
   </sheetPr>
   <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2616,7 +2747,7 @@
       </c>
       <c r="U6" s="37">
         <f>COUNTIF(H2:H89,"*Passed*")</f>
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="70" x14ac:dyDescent="0.35">
@@ -2915,7 +3046,7 @@
         <v>33</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="M14" s="31">
         <v>42082</v>
@@ -3151,7 +3282,7 @@
         <v>33</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="M20" s="39">
         <v>42104</v>
@@ -3349,7 +3480,7 @@
       </c>
       <c r="U25" s="29">
         <f>COUNTIF(L2:L49,"*Minor*")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="58" x14ac:dyDescent="0.35">
@@ -3402,15 +3533,37 @@
       </c>
       <c r="U26" s="29">
         <f>COUNTIF(L2:L26,"*Moderate*")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="56" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="32">
+        <v>42109</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
@@ -3426,12 +3579,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="8"/>
+    <row r="28" spans="1:21" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="32">
+        <v>42109</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
@@ -3447,12 +3622,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="8"/>
+    <row r="29" spans="1:21" ht="58" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B29" s="41" t="s">
+        <v>266</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="32">
+        <v>42109</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
@@ -3469,6 +3666,7 @@
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
       <c r="G30" s="8"/>
@@ -5350,10 +5548,10 @@
   <sheetPr>
     <tabColor rgb="FF99FF99"/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5971,6 +6169,78 @@
       <c r="E27" s="38" t="s">
         <v>252</v>
       </c>
+    </row>
+    <row r="28" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="38" t="s">
+        <v>267</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>269</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>270</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="38" t="s">
+        <v>268</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>271</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>272</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>273</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="38" t="s">
+        <v>275</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>276</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35" s="3"/>
+      <c r="C35" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6064,18 +6334,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6193,6 +6463,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -6203,14 +6481,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>